<commit_message>
finaly working now Médias a funcionar
</commit_message>
<xml_diff>
--- a/ExcelVoice/IM_Excel/ETP3.xlsx
+++ b/ExcelVoice/IM_Excel/ETP3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae9757b855731a8f/Desktop/IM_EXCEL_Projects/ExcelVoice/IM_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7569" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790349DE-D643-457D-8C61-A40836273E5C}"/>
+  <xr:revisionPtr revIDLastSave="8319" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CBBCE8-FEF9-4C2A-AA9B-D810F8082506}"/>
   <bookViews>
-    <workbookView xWindow="5316" yWindow="336" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2394,6 +2394,10 @@
       <c r="O3">
         <v>2</v>
       </c>
+      <c r="P3">
+        <f>AVERAGE(H3,N3,O3)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">

</xml_diff>

<commit_message>
melhoria quse a funcionar
</commit_message>
<xml_diff>
--- a/ExcelVoice/IM_Excel/ETP3.xlsx
+++ b/ExcelVoice/IM_Excel/ETP3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae9757b855731a8f/Desktop/IM_EXCEL_Projects/ExcelVoice/IM_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8319" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CBBCE8-FEF9-4C2A-AA9B-D810F8082506}"/>
+  <xr:revisionPtr revIDLastSave="10093" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFAE0436-D498-4E46-B2A5-5B02AC34E5A9}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="354">
   <si>
     <t>Número mecanográfico</t>
   </si>
@@ -1086,6 +1086,15 @@
   </si>
   <si>
     <t>Média</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1119,6 +1128,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF08080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1170,6 +1191,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,15 +2262,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P160"/>
+  <dimension ref="A1:Q160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,8 +2319,11 @@
       <c r="P1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>107447</v>
       </c>
@@ -2347,8 +2373,11 @@
         <f>AVERAGE(H2,N2,O2)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>94716</v>
       </c>
@@ -2398,8 +2427,11 @@
         <f>AVERAGE(H3,N3,O3)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>107135</v>
       </c>
@@ -2445,8 +2477,15 @@
       <c r="O4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <f>AVERAGE(H4,N4,O4)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>107390</v>
       </c>
@@ -2486,8 +2525,15 @@
       <c r="O5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P5" s="2">
+        <f>AVERAGE(H5,N5,O5)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>108121</v>
       </c>
@@ -2533,8 +2579,15 @@
       <c r="O6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <f>AVERAGE(H6,N6,O6)</f>
+        <v>8</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107242</v>
       </c>
@@ -2580,8 +2633,15 @@
       <c r="O7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <f>AVERAGE(H7,N7,O7)</f>
+        <v>10</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>108589</v>
       </c>
@@ -2627,8 +2687,15 @@
       <c r="O8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <f>AVERAGE(H8,N8,O8)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108522</v>
       </c>
@@ -2674,8 +2741,15 @@
       <c r="O9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <f>AVERAGE(H9,N9,O9)</f>
+        <v>11</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>107218</v>
       </c>
@@ -2721,8 +2795,15 @@
       <c r="O10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P10" s="2">
+        <f>AVERAGE(H10,N10,O10)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>108189</v>
       </c>
@@ -2768,8 +2849,15 @@
       <c r="O11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <f>AVERAGE(H11,N11,O11)</f>
+        <v>9</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>107372</v>
       </c>
@@ -2815,8 +2903,15 @@
       <c r="O12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <f>AVERAGE(H12,N12,O12)</f>
+        <v>11</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>108957</v>
       </c>
@@ -2862,8 +2957,15 @@
       <c r="O13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <f>AVERAGE(H13,N13,O13)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>107440</v>
       </c>
@@ -2909,8 +3011,15 @@
       <c r="O14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <f>AVERAGE(H14,N14,O14)</f>
+        <v>11</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>108188</v>
       </c>
@@ -2956,8 +3065,15 @@
       <c r="O15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <f>AVERAGE(H15,N15,O15)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>108855</v>
       </c>
@@ -3003,8 +3119,15 @@
       <c r="O16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <f>AVERAGE(H16,N16,O16)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>108672</v>
       </c>
@@ -3050,8 +3173,15 @@
       <c r="O17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <f>AVERAGE(H17,N17,O17)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>108138</v>
       </c>
@@ -3097,8 +3227,15 @@
       <c r="O18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <f>AVERAGE(H18,N18,O18)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>107236</v>
       </c>
@@ -3144,8 +3281,15 @@
       <c r="O19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <f>AVERAGE(H19,N19,O19)</f>
+        <v>8</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>104204</v>
       </c>
@@ -3191,8 +3335,15 @@
       <c r="O20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <f>AVERAGE(H20,N20,O20)</f>
+        <v>12</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>107428</v>
       </c>
@@ -3238,8 +3389,15 @@
       <c r="O21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <f>AVERAGE(H21,N21,O21)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>107259</v>
       </c>
@@ -3285,8 +3443,15 @@
       <c r="O22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="2">
+        <f>AVERAGE(H22,N22,O22)</f>
+        <v>8</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100088</v>
       </c>
@@ -3332,8 +3497,15 @@
       <c r="O23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <f>AVERAGE(H23,N23,O23)</f>
+        <v>9</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>108506</v>
       </c>
@@ -3379,8 +3551,15 @@
       <c r="O24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <f>AVERAGE(H24,N24,O24)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>110376</v>
       </c>
@@ -3426,8 +3605,15 @@
       <c r="O25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <f>AVERAGE(H25,N25,O25)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>109038</v>
       </c>
@@ -3473,8 +3659,15 @@
       <c r="O26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <f>AVERAGE(H26,N26,O26)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>108727</v>
       </c>
@@ -3520,8 +3713,15 @@
       <c r="O27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <f>AVERAGE(H27,N27,O27)</f>
+        <v>7</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>93973</v>
       </c>
@@ -3567,8 +3767,15 @@
       <c r="O28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <f>AVERAGE(H28,N28,O28)</f>
+        <v>8</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>108381</v>
       </c>
@@ -3614,8 +3821,15 @@
       <c r="O29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="2">
+        <f>AVERAGE(H29,N29,O29)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>108694</v>
       </c>
@@ -3661,8 +3875,15 @@
       <c r="O30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="2">
+        <f>AVERAGE(H30,N30,O30)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>108421</v>
       </c>
@@ -3708,8 +3929,15 @@
       <c r="O31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <f>AVERAGE(H31,N31,O31)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>108366</v>
       </c>
@@ -3755,8 +3983,15 @@
       <c r="O32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="2">
+        <f>AVERAGE(H32,N32,O32)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>109462</v>
       </c>
@@ -3802,8 +4037,15 @@
       <c r="O33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <f>AVERAGE(H33,N33,O33)</f>
+        <v>8</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>93742</v>
       </c>
@@ -3849,8 +4091,15 @@
       <c r="O34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <f>AVERAGE(H34,N34,O34)</f>
+        <v>9</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>109000</v>
       </c>
@@ -3896,8 +4145,15 @@
       <c r="O35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <f>AVERAGE(H35,N35,O35)</f>
+        <v>11</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>107769</v>
       </c>
@@ -3943,8 +4199,15 @@
       <c r="O36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P36" s="2">
+        <f>AVERAGE(H36,N36,O36)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>101446</v>
       </c>
@@ -3990,8 +4253,15 @@
       <c r="O37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="2">
+        <f>AVERAGE(H37,N37,O37)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>109061</v>
       </c>
@@ -4037,8 +4307,15 @@
       <c r="O38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <f>AVERAGE(H38,N38,O38)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>107487</v>
       </c>
@@ -4084,8 +4361,15 @@
       <c r="O39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <f>AVERAGE(H39,N39,O39)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>107436</v>
       </c>
@@ -4131,8 +4415,15 @@
       <c r="O40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <f>AVERAGE(H40,N40,O40)</f>
+        <v>10</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>107529</v>
       </c>
@@ -4178,8 +4469,15 @@
       <c r="O41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="2">
+        <f>AVERAGE(H41,N41,O41)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>107879</v>
       </c>
@@ -4225,8 +4523,15 @@
       <c r="O42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="2">
+        <f>AVERAGE(H42,N42,O42)</f>
+        <v>8</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>107788</v>
       </c>
@@ -4272,8 +4577,15 @@
       <c r="O43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <f>AVERAGE(H43,N43,O43)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>108449</v>
       </c>
@@ -4319,8 +4631,15 @@
       <c r="O44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <f>AVERAGE(H44,N44,O44)</f>
+        <v>9</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>108651</v>
       </c>
@@ -4366,8 +4685,15 @@
       <c r="O45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="2">
+        <f>AVERAGE(H45,N45,O45)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>107560</v>
       </c>
@@ -4413,8 +4739,15 @@
       <c r="O46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <f>AVERAGE(H46,N46,O46)</f>
+        <v>13</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>107977</v>
       </c>
@@ -4460,8 +4793,15 @@
       <c r="O47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <f>AVERAGE(H47,N47,O47)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>107369</v>
       </c>
@@ -4507,8 +4847,15 @@
       <c r="O48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <f>AVERAGE(H48,N48,O48)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>108171</v>
       </c>
@@ -4554,8 +4901,15 @@
       <c r="O49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <f>AVERAGE(H49,N49,O49)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q49" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>107920</v>
       </c>
@@ -4601,8 +4955,15 @@
       <c r="O50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <f>AVERAGE(H50,N50,O50)</f>
+        <v>7</v>
+      </c>
+      <c r="Q50" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>109342</v>
       </c>
@@ -4648,8 +5009,15 @@
       <c r="O51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P51">
+        <f>AVERAGE(H51,N51,O51)</f>
+        <v>9</v>
+      </c>
+      <c r="Q51" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>108430</v>
       </c>
@@ -4695,8 +5063,15 @@
       <c r="O52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P52" s="2">
+        <f>AVERAGE(H52,N52,O52)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q52" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>108816</v>
       </c>
@@ -4742,8 +5117,15 @@
       <c r="O53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P53" s="2">
+        <f>AVERAGE(H53,N53,O53)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>108842</v>
       </c>
@@ -4789,8 +5171,15 @@
       <c r="O54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54" s="2">
+        <f>AVERAGE(H54,N54,O54)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>103797</v>
       </c>
@@ -4836,8 +5225,15 @@
       <c r="O55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55">
+        <f>AVERAGE(H55,N55,O55)</f>
+        <v>8</v>
+      </c>
+      <c r="Q55" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>107777</v>
       </c>
@@ -4883,8 +5279,15 @@
       <c r="O56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56">
+        <f>AVERAGE(H56,N56,O56)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q56" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>107717</v>
       </c>
@@ -4930,8 +5333,15 @@
       <c r="O57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57">
+        <f>AVERAGE(H57,N57,O57)</f>
+        <v>9</v>
+      </c>
+      <c r="Q57" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>103443</v>
       </c>
@@ -4977,8 +5387,15 @@
       <c r="O58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58">
+        <f>AVERAGE(H58,N58,O58)</f>
+        <v>10</v>
+      </c>
+      <c r="Q58" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>108950</v>
       </c>
@@ -5024,8 +5441,15 @@
       <c r="O59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59">
+        <f>AVERAGE(H59,N59,O59)</f>
+        <v>12</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>108079</v>
       </c>
@@ -5071,8 +5495,15 @@
       <c r="O60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P60">
+        <f>AVERAGE(H60,N60,O60)</f>
+        <v>7</v>
+      </c>
+      <c r="Q60" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>109163</v>
       </c>
@@ -5118,8 +5549,15 @@
       <c r="O61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61" s="2">
+        <f>AVERAGE(H61,N61,O61)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q61" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>110347</v>
       </c>
@@ -5165,8 +5603,15 @@
       <c r="O62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62">
+        <f>AVERAGE(H62,N62,O62)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q62" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>109373</v>
       </c>
@@ -5212,8 +5657,15 @@
       <c r="O63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63">
+        <f>AVERAGE(H63,N63,O63)</f>
+        <v>10</v>
+      </c>
+      <c r="Q63" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>103203</v>
       </c>
@@ -5259,8 +5711,15 @@
       <c r="O64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64">
+        <f>AVERAGE(H64,N64,O64)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q64" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>107335</v>
       </c>
@@ -5306,8 +5765,15 @@
       <c r="O65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65">
+        <f>AVERAGE(H65,N65,O65)</f>
+        <v>11</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>93345</v>
       </c>
@@ -5353,8 +5819,15 @@
       <c r="O66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66">
+        <f>AVERAGE(H66,N66,O66)</f>
+        <v>12</v>
+      </c>
+      <c r="Q66" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>103409</v>
       </c>
@@ -5400,8 +5873,15 @@
       <c r="O67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P67">
+        <f>AVERAGE(H67,N67,O67)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q67" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>108105</v>
       </c>
@@ -5447,8 +5927,15 @@
       <c r="O68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" s="2">
+        <f>AVERAGE(H68,N68,O68)</f>
+        <v>10</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>107848</v>
       </c>
@@ -5494,8 +5981,15 @@
       <c r="O69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69">
+        <f>AVERAGE(H69,N69,O69)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q69" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>107318</v>
       </c>
@@ -5541,8 +6035,15 @@
       <c r="O70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70">
+        <f>AVERAGE(H70,N70,O70)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q70" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>107611</v>
       </c>
@@ -5588,8 +6089,15 @@
       <c r="O71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71">
+        <f>AVERAGE(H71,N71,O71)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q71" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>108845</v>
       </c>
@@ -5635,8 +6143,15 @@
       <c r="O72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P72">
+        <f>AVERAGE(H72,N72,O72)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q72" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>108098</v>
       </c>
@@ -5682,8 +6197,15 @@
       <c r="O73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P73">
+        <f>AVERAGE(H73,N73,O73)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q73" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>108723</v>
       </c>
@@ -5729,8 +6251,15 @@
       <c r="O74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P74">
+        <f>AVERAGE(H74,N74,O74)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q74" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>103757</v>
       </c>
@@ -5776,8 +6305,15 @@
       <c r="O75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P75">
+        <f>AVERAGE(H75,N75,O75)</f>
+        <v>8</v>
+      </c>
+      <c r="Q75" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>107396</v>
       </c>
@@ -5823,8 +6359,15 @@
       <c r="O76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P76">
+        <f>AVERAGE(H76,N76,O76)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>108675</v>
       </c>
@@ -5870,8 +6413,15 @@
       <c r="O77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P77">
+        <f>AVERAGE(H77,N77,O77)</f>
+        <v>8</v>
+      </c>
+      <c r="Q77" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>107584</v>
       </c>
@@ -5917,8 +6467,15 @@
       <c r="O78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P78">
+        <f>AVERAGE(H78,N78,O78)</f>
+        <v>9</v>
+      </c>
+      <c r="Q78" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>108329</v>
       </c>
@@ -5964,8 +6521,15 @@
       <c r="O79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P79">
+        <f>AVERAGE(H79,N79,O79)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q79" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>107874</v>
       </c>
@@ -6011,8 +6575,15 @@
       <c r="O80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80">
+        <f>AVERAGE(H80,N80,O80)</f>
+        <v>10</v>
+      </c>
+      <c r="Q80" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>107517</v>
       </c>
@@ -6058,8 +6629,15 @@
       <c r="O81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81">
+        <f>AVERAGE(H81,N81,O81)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q81" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>108513</v>
       </c>
@@ -6105,8 +6683,15 @@
       <c r="O82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82">
+        <f>AVERAGE(H82,N82,O82)</f>
+        <v>10</v>
+      </c>
+      <c r="Q82" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>104342</v>
       </c>
@@ -6152,8 +6737,15 @@
       <c r="O83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83">
+        <f>AVERAGE(H83,N83,O83)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q83" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>108752</v>
       </c>
@@ -6199,8 +6791,15 @@
       <c r="O84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84">
+        <f>AVERAGE(H84,N84,O84)</f>
+        <v>10</v>
+      </c>
+      <c r="Q84" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>103712</v>
       </c>
@@ -6246,8 +6845,15 @@
       <c r="O85">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85">
+        <f>AVERAGE(H85,N85,O85)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q85" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>108849</v>
       </c>
@@ -6293,8 +6899,15 @@
       <c r="O86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P86">
+        <f>AVERAGE(H86,N86,O86)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>108868</v>
       </c>
@@ -6340,8 +6953,15 @@
       <c r="O87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87" s="2">
+        <f>AVERAGE(H87,N87,O87)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q87" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>102380</v>
       </c>
@@ -6387,8 +7007,15 @@
       <c r="O88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88">
+        <f>AVERAGE(H88,N88,O88)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>107265</v>
       </c>
@@ -6434,8 +7061,15 @@
       <c r="O89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89">
+        <f>AVERAGE(H89,N89,O89)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>108280</v>
       </c>
@@ -6481,8 +7115,15 @@
       <c r="O90">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P90">
+        <f>AVERAGE(H90,N90,O90)</f>
+        <v>8</v>
+      </c>
+      <c r="Q90" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>97610</v>
       </c>
@@ -6528,8 +7169,15 @@
       <c r="O91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91" s="2">
+        <f>AVERAGE(H91,N91,O91)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q91" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>93316</v>
       </c>
@@ -6575,8 +7223,15 @@
       <c r="O92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92">
+        <f>AVERAGE(H92,N92,O92)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q92" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>110331</v>
       </c>
@@ -6622,8 +7277,15 @@
       <c r="O93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P93">
+        <f>AVERAGE(H93,N93,O93)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q93" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>104807</v>
       </c>
@@ -6669,8 +7331,15 @@
       <c r="O94">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94">
+        <f>AVERAGE(H94,N94,O94)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q94" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>108679</v>
       </c>
@@ -6716,8 +7385,15 @@
       <c r="O95">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P95">
+        <f>AVERAGE(H95,N95,O95)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q95" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>103028</v>
       </c>
@@ -6763,8 +7439,15 @@
       <c r="O96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96" s="2">
+        <f>AVERAGE(H96,N96,O96)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q96" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>105114</v>
       </c>
@@ -6810,8 +7493,15 @@
       <c r="O97">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P97">
+        <f>AVERAGE(H97,N97,O97)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q97" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>108800</v>
       </c>
@@ -6857,8 +7547,15 @@
       <c r="O98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P98" s="2">
+        <f>AVERAGE(H98,N98,O98)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q98" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>108050</v>
       </c>
@@ -6904,8 +7601,15 @@
       <c r="O99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P99">
+        <f>AVERAGE(H99,N99,O99)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q99" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>105491</v>
       </c>
@@ -6951,8 +7655,15 @@
       <c r="O100">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P100">
+        <f>AVERAGE(H100,N100,O100)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>102976</v>
       </c>
@@ -6998,8 +7709,15 @@
       <c r="O101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P101" s="2">
+        <f>AVERAGE(H101,N101,O101)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q101" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>108826</v>
       </c>
@@ -7045,8 +7763,15 @@
       <c r="O102">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P102">
+        <f>AVERAGE(H102,N102,O102)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>108436</v>
       </c>
@@ -7092,8 +7817,15 @@
       <c r="O103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P103" s="2">
+        <f>AVERAGE(H103,N103,O103)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q103" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>107233</v>
       </c>
@@ -7139,8 +7871,15 @@
       <c r="O104">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P104" s="2">
+        <f>AVERAGE(H104,N104,O104)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103167</v>
       </c>
@@ -7186,8 +7925,15 @@
       <c r="O105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P105">
+        <f>AVERAGE(H105,N105,O105)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q105" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>108760</v>
       </c>
@@ -7233,8 +7979,15 @@
       <c r="O106">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P106">
+        <f>AVERAGE(H106,N106,O106)</f>
+        <v>7</v>
+      </c>
+      <c r="Q106" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>103326</v>
       </c>
@@ -7280,8 +8033,15 @@
       <c r="O107">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P107" s="2">
+        <f>AVERAGE(H107,N107,O107)</f>
+        <v>10</v>
+      </c>
+      <c r="Q107" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>109152</v>
       </c>
@@ -7327,8 +8087,15 @@
       <c r="O108">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P108">
+        <f>AVERAGE(H108,N108,O108)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q108" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107895</v>
       </c>
@@ -7374,8 +8141,15 @@
       <c r="O109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P109">
+        <f>AVERAGE(H109,N109,O109)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q109" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>107267</v>
       </c>
@@ -7421,8 +8195,15 @@
       <c r="O110">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P110">
+        <f>AVERAGE(H110,N110,O110)</f>
+        <v>8</v>
+      </c>
+      <c r="Q110" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>103309</v>
       </c>
@@ -7468,8 +8249,15 @@
       <c r="O111">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P111">
+        <f>AVERAGE(H111,N111,O111)</f>
+        <v>9</v>
+      </c>
+      <c r="Q111" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>99440</v>
       </c>
@@ -7515,8 +8303,15 @@
       <c r="O112">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P112" s="2">
+        <f>AVERAGE(H112,N112,O112)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q112" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>93274</v>
       </c>
@@ -7562,8 +8357,15 @@
       <c r="O113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P113">
+        <f>AVERAGE(H113,N113,O113)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q113" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>102859</v>
       </c>
@@ -7609,8 +8411,15 @@
       <c r="O114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P114">
+        <f>AVERAGE(H114,N114,O114)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q114" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>104088</v>
       </c>
@@ -7656,8 +8465,15 @@
       <c r="O115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P115">
+        <f>AVERAGE(H115,N115,O115)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q115" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>102633</v>
       </c>
@@ -7703,8 +8519,15 @@
       <c r="O116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P116">
+        <f>AVERAGE(H116,N116,O116)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q116" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>108159</v>
       </c>
@@ -7750,8 +8573,15 @@
       <c r="O117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P117">
+        <f>AVERAGE(H117,N117,O117)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q117" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>108461</v>
       </c>
@@ -7797,8 +8627,15 @@
       <c r="O118">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P118" s="2">
+        <f>AVERAGE(H118,N118,O118)</f>
+        <v>10</v>
+      </c>
+      <c r="Q118" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>107635</v>
       </c>
@@ -7844,8 +8681,15 @@
       <c r="O119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P119">
+        <f>AVERAGE(H119,N119,O119)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q119" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>102716</v>
       </c>
@@ -7891,8 +8735,15 @@
       <c r="O120">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P120">
+        <f>AVERAGE(H120,N120,O120)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q120" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>107347</v>
       </c>
@@ -7938,8 +8789,15 @@
       <c r="O121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P121">
+        <f>AVERAGE(H121,N121,O121)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q121" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>110409</v>
       </c>
@@ -7985,8 +8843,15 @@
       <c r="O122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P122">
+        <f>AVERAGE(H122,N122,O122)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q122" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>108540</v>
       </c>
@@ -8032,8 +8897,15 @@
       <c r="O123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P123" s="2">
+        <f>AVERAGE(H123,N123,O123)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q123" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>103112</v>
       </c>
@@ -8079,8 +8951,15 @@
       <c r="O124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P124">
+        <f>AVERAGE(H124,N124,O124)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q124" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>111224</v>
       </c>
@@ -8126,8 +9005,15 @@
       <c r="O125">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P125">
+        <f>AVERAGE(H125,N125,O125)</f>
+        <v>9</v>
+      </c>
+      <c r="Q125" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>102150</v>
       </c>
@@ -8173,8 +9059,15 @@
       <c r="O126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P126" s="2">
+        <f>AVERAGE(H126,N126,O126)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q126" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>107185</v>
       </c>
@@ -8220,8 +9113,15 @@
       <c r="O127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P127">
+        <f>AVERAGE(H127,N127,O127)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q127" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>104229</v>
       </c>
@@ -8267,8 +9167,15 @@
       <c r="O128">
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P128">
+        <f>AVERAGE(H128,N128,O128)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q128" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>103235</v>
       </c>
@@ -8314,8 +9221,15 @@
       <c r="O129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P129">
+        <f>AVERAGE(H129,N129,O129)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q129" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>110719</v>
       </c>
@@ -8361,8 +9275,15 @@
       <c r="O130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P130">
+        <f>AVERAGE(H130,N130,O130)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q130" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>102669</v>
       </c>
@@ -8408,8 +9329,15 @@
       <c r="O131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P131">
+        <f>AVERAGE(H131,N131,O131)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q131" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>108113</v>
       </c>
@@ -8455,8 +9383,15 @@
       <c r="O132">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P132">
+        <f>AVERAGE(H132,N132,O132)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q132" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>108204</v>
       </c>
@@ -8502,8 +9437,15 @@
       <c r="O133">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P133">
+        <f>AVERAGE(H133,N133,O133)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q133" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>107356</v>
       </c>
@@ -8549,8 +9491,15 @@
       <c r="O134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P134">
+        <f>AVERAGE(H134,N134,O134)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q134" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>102011</v>
       </c>
@@ -8596,8 +9545,15 @@
       <c r="O135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P135">
+        <f>AVERAGE(H135,N135,O135)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q135" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>104183</v>
       </c>
@@ -8643,8 +9599,15 @@
       <c r="O136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P136">
+        <f>AVERAGE(H136,N136,O136)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q136" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>108629</v>
       </c>
@@ -8690,8 +9653,15 @@
       <c r="O137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P137">
+        <f>AVERAGE(H137,N137,O137)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q137" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>102743</v>
       </c>
@@ -8737,8 +9707,15 @@
       <c r="O138">
         <v>2</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P138" s="2">
+        <f>AVERAGE(H138,N138,O138)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q138" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>108654</v>
       </c>
@@ -8784,8 +9761,15 @@
       <c r="O139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P139">
+        <f>AVERAGE(H139,N139,O139)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q139" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>108869</v>
       </c>
@@ -8831,8 +9815,15 @@
       <c r="O140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P140">
+        <f>AVERAGE(H140,N140,O140)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q140" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>103761</v>
       </c>
@@ -8878,8 +9869,15 @@
       <c r="O141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P141" s="2">
+        <f>AVERAGE(H141,N141,O141)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q141" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>107208</v>
       </c>
@@ -8925,8 +9923,15 @@
       <c r="O142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P142">
+        <f>AVERAGE(H142,N142,O142)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q142" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>103314</v>
       </c>
@@ -8972,8 +9977,15 @@
       <c r="O143">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P143" s="2">
+        <f>AVERAGE(H143,N143,O143)</f>
+        <v>8</v>
+      </c>
+      <c r="Q143" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>109150</v>
       </c>
@@ -9019,8 +10031,15 @@
       <c r="O144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P144">
+        <f>AVERAGE(H144,N144,O144)</f>
+        <v>10</v>
+      </c>
+      <c r="Q144" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>105431</v>
       </c>
@@ -9066,8 +10085,15 @@
       <c r="O145">
         <v>2</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P145" s="2">
+        <f>AVERAGE(H145,N145,O145)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q145" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>103768</v>
       </c>
@@ -9113,8 +10139,15 @@
       <c r="O146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P146">
+        <f>AVERAGE(H146,N146,O146)</f>
+        <v>11</v>
+      </c>
+      <c r="Q146" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>98007</v>
       </c>
@@ -9160,8 +10193,15 @@
       <c r="O147">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P147">
+        <f>AVERAGE(H147,N147,O147)</f>
+        <v>7</v>
+      </c>
+      <c r="Q147" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>107594</v>
       </c>
@@ -9207,8 +10247,15 @@
       <c r="O148">
         <v>2</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P148">
+        <f>AVERAGE(H148,N148,O148)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q148" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>107319</v>
       </c>
@@ -9254,8 +10301,15 @@
       <c r="O149">
         <v>2</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P149">
+        <f>AVERAGE(H149,N149,O149)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q149" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>99397</v>
       </c>
@@ -9301,8 +10355,15 @@
       <c r="O150">
         <v>2</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P150">
+        <f>AVERAGE(H150,N150,O150)</f>
+        <v>9</v>
+      </c>
+      <c r="Q150" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>105127</v>
       </c>
@@ -9348,8 +10409,15 @@
       <c r="O151">
         <v>2</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P151" s="2">
+        <f>AVERAGE(H151,N151,O151)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q151" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>105083</v>
       </c>
@@ -9395,8 +10463,15 @@
       <c r="O152">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P152" s="2">
+        <f>AVERAGE(H152,N152,O152)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q152" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>109162</v>
       </c>
@@ -9442,8 +10517,15 @@
       <c r="O153">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P153">
+        <f>AVERAGE(H153,N153,O153)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q153" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>108225</v>
       </c>
@@ -9489,8 +10571,15 @@
       <c r="O154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P154">
+        <f>AVERAGE(H154,N154,O154)</f>
+        <v>6</v>
+      </c>
+      <c r="Q154" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105880</v>
       </c>
@@ -9536,8 +10625,15 @@
       <c r="O155">
         <v>2</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P155">
+        <f>AVERAGE(H155,N155,O155)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q155" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>108078</v>
       </c>
@@ -9583,8 +10679,15 @@
       <c r="O156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P156">
+        <f>AVERAGE(H156,N156,O156)</f>
+        <v>10</v>
+      </c>
+      <c r="Q156" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>108146</v>
       </c>
@@ -9630,8 +10733,15 @@
       <c r="O157">
         <v>2</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P157" s="2">
+        <f>AVERAGE(H157,N157,O157)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q157" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>102437</v>
       </c>
@@ -9677,8 +10787,15 @@
       <c r="O158">
         <v>2</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P158">
+        <f>AVERAGE(H158,N158,O158)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q158" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>97876</v>
       </c>
@@ -9724,8 +10841,15 @@
       <c r="O159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P159">
+        <f>AVERAGE(H159,N159,O159)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q159" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>103910</v>
       </c>
@@ -9770,6 +10894,13 @@
       </c>
       <c r="O160">
         <v>2</v>
+      </c>
+      <c r="P160">
+        <f>AVERAGE(H160,N160,O160)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q160" s="5" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
melhorias na interface do index.html
</commit_message>
<xml_diff>
--- a/ExcelVoice/IM_Excel/ETP3.xlsx
+++ b/ExcelVoice/IM_Excel/ETP3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae9757b855731a8f/Desktop/IM_EXCEL_Projects/ExcelVoice/IM_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8319" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CBBCE8-FEF9-4C2A-AA9B-D810F8082506}"/>
+  <xr:revisionPtr revIDLastSave="10093" documentId="13_ncr:1_{7CC2716A-D035-4DD3-A189-8164E5F19EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFAE0436-D498-4E46-B2A5-5B02AC34E5A9}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="354">
   <si>
     <t>Número mecanográfico</t>
   </si>
@@ -1086,6 +1086,15 @@
   </si>
   <si>
     <t>Média</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1119,6 +1128,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF08080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1170,6 +1191,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,15 +2262,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P160"/>
+  <dimension ref="A1:Q160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,8 +2319,11 @@
       <c r="P1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>107447</v>
       </c>
@@ -2347,8 +2373,11 @@
         <f>AVERAGE(H2,N2,O2)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>94716</v>
       </c>
@@ -2398,8 +2427,11 @@
         <f>AVERAGE(H3,N3,O3)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>107135</v>
       </c>
@@ -2445,8 +2477,15 @@
       <c r="O4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <f>AVERAGE(H4,N4,O4)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>107390</v>
       </c>
@@ -2486,8 +2525,15 @@
       <c r="O5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P5" s="2">
+        <f>AVERAGE(H5,N5,O5)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>108121</v>
       </c>
@@ -2533,8 +2579,15 @@
       <c r="O6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <f>AVERAGE(H6,N6,O6)</f>
+        <v>8</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107242</v>
       </c>
@@ -2580,8 +2633,15 @@
       <c r="O7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <f>AVERAGE(H7,N7,O7)</f>
+        <v>10</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>108589</v>
       </c>
@@ -2627,8 +2687,15 @@
       <c r="O8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <f>AVERAGE(H8,N8,O8)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108522</v>
       </c>
@@ -2674,8 +2741,15 @@
       <c r="O9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <f>AVERAGE(H9,N9,O9)</f>
+        <v>11</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>107218</v>
       </c>
@@ -2721,8 +2795,15 @@
       <c r="O10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P10" s="2">
+        <f>AVERAGE(H10,N10,O10)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>108189</v>
       </c>
@@ -2768,8 +2849,15 @@
       <c r="O11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <f>AVERAGE(H11,N11,O11)</f>
+        <v>9</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>107372</v>
       </c>
@@ -2815,8 +2903,15 @@
       <c r="O12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <f>AVERAGE(H12,N12,O12)</f>
+        <v>11</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>108957</v>
       </c>
@@ -2862,8 +2957,15 @@
       <c r="O13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <f>AVERAGE(H13,N13,O13)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>107440</v>
       </c>
@@ -2909,8 +3011,15 @@
       <c r="O14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <f>AVERAGE(H14,N14,O14)</f>
+        <v>11</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>108188</v>
       </c>
@@ -2956,8 +3065,15 @@
       <c r="O15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <f>AVERAGE(H15,N15,O15)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>108855</v>
       </c>
@@ -3003,8 +3119,15 @@
       <c r="O16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <f>AVERAGE(H16,N16,O16)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>108672</v>
       </c>
@@ -3050,8 +3173,15 @@
       <c r="O17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <f>AVERAGE(H17,N17,O17)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>108138</v>
       </c>
@@ -3097,8 +3227,15 @@
       <c r="O18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <f>AVERAGE(H18,N18,O18)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>107236</v>
       </c>
@@ -3144,8 +3281,15 @@
       <c r="O19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <f>AVERAGE(H19,N19,O19)</f>
+        <v>8</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>104204</v>
       </c>
@@ -3191,8 +3335,15 @@
       <c r="O20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <f>AVERAGE(H20,N20,O20)</f>
+        <v>12</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>107428</v>
       </c>
@@ -3238,8 +3389,15 @@
       <c r="O21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <f>AVERAGE(H21,N21,O21)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>107259</v>
       </c>
@@ -3285,8 +3443,15 @@
       <c r="O22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="2">
+        <f>AVERAGE(H22,N22,O22)</f>
+        <v>8</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100088</v>
       </c>
@@ -3332,8 +3497,15 @@
       <c r="O23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <f>AVERAGE(H23,N23,O23)</f>
+        <v>9</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>108506</v>
       </c>
@@ -3379,8 +3551,15 @@
       <c r="O24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <f>AVERAGE(H24,N24,O24)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>110376</v>
       </c>
@@ -3426,8 +3605,15 @@
       <c r="O25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <f>AVERAGE(H25,N25,O25)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>109038</v>
       </c>
@@ -3473,8 +3659,15 @@
       <c r="O26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <f>AVERAGE(H26,N26,O26)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>108727</v>
       </c>
@@ -3520,8 +3713,15 @@
       <c r="O27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <f>AVERAGE(H27,N27,O27)</f>
+        <v>7</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>93973</v>
       </c>
@@ -3567,8 +3767,15 @@
       <c r="O28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <f>AVERAGE(H28,N28,O28)</f>
+        <v>8</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>108381</v>
       </c>
@@ -3614,8 +3821,15 @@
       <c r="O29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="2">
+        <f>AVERAGE(H29,N29,O29)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>108694</v>
       </c>
@@ -3661,8 +3875,15 @@
       <c r="O30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="2">
+        <f>AVERAGE(H30,N30,O30)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>108421</v>
       </c>
@@ -3708,8 +3929,15 @@
       <c r="O31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <f>AVERAGE(H31,N31,O31)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>108366</v>
       </c>
@@ -3755,8 +3983,15 @@
       <c r="O32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="2">
+        <f>AVERAGE(H32,N32,O32)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>109462</v>
       </c>
@@ -3802,8 +4037,15 @@
       <c r="O33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <f>AVERAGE(H33,N33,O33)</f>
+        <v>8</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>93742</v>
       </c>
@@ -3849,8 +4091,15 @@
       <c r="O34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <f>AVERAGE(H34,N34,O34)</f>
+        <v>9</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>109000</v>
       </c>
@@ -3896,8 +4145,15 @@
       <c r="O35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <f>AVERAGE(H35,N35,O35)</f>
+        <v>11</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>107769</v>
       </c>
@@ -3943,8 +4199,15 @@
       <c r="O36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P36" s="2">
+        <f>AVERAGE(H36,N36,O36)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>101446</v>
       </c>
@@ -3990,8 +4253,15 @@
       <c r="O37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="2">
+        <f>AVERAGE(H37,N37,O37)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>109061</v>
       </c>
@@ -4037,8 +4307,15 @@
       <c r="O38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <f>AVERAGE(H38,N38,O38)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>107487</v>
       </c>
@@ -4084,8 +4361,15 @@
       <c r="O39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <f>AVERAGE(H39,N39,O39)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>107436</v>
       </c>
@@ -4131,8 +4415,15 @@
       <c r="O40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <f>AVERAGE(H40,N40,O40)</f>
+        <v>10</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>107529</v>
       </c>
@@ -4178,8 +4469,15 @@
       <c r="O41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="2">
+        <f>AVERAGE(H41,N41,O41)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>107879</v>
       </c>
@@ -4225,8 +4523,15 @@
       <c r="O42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="2">
+        <f>AVERAGE(H42,N42,O42)</f>
+        <v>8</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>107788</v>
       </c>
@@ -4272,8 +4577,15 @@
       <c r="O43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <f>AVERAGE(H43,N43,O43)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>108449</v>
       </c>
@@ -4319,8 +4631,15 @@
       <c r="O44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <f>AVERAGE(H44,N44,O44)</f>
+        <v>9</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>108651</v>
       </c>
@@ -4366,8 +4685,15 @@
       <c r="O45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="2">
+        <f>AVERAGE(H45,N45,O45)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>107560</v>
       </c>
@@ -4413,8 +4739,15 @@
       <c r="O46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <f>AVERAGE(H46,N46,O46)</f>
+        <v>13</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>107977</v>
       </c>
@@ -4460,8 +4793,15 @@
       <c r="O47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <f>AVERAGE(H47,N47,O47)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>107369</v>
       </c>
@@ -4507,8 +4847,15 @@
       <c r="O48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <f>AVERAGE(H48,N48,O48)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>108171</v>
       </c>
@@ -4554,8 +4901,15 @@
       <c r="O49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <f>AVERAGE(H49,N49,O49)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q49" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>107920</v>
       </c>
@@ -4601,8 +4955,15 @@
       <c r="O50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <f>AVERAGE(H50,N50,O50)</f>
+        <v>7</v>
+      </c>
+      <c r="Q50" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>109342</v>
       </c>
@@ -4648,8 +5009,15 @@
       <c r="O51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P51">
+        <f>AVERAGE(H51,N51,O51)</f>
+        <v>9</v>
+      </c>
+      <c r="Q51" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>108430</v>
       </c>
@@ -4695,8 +5063,15 @@
       <c r="O52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P52" s="2">
+        <f>AVERAGE(H52,N52,O52)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q52" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>108816</v>
       </c>
@@ -4742,8 +5117,15 @@
       <c r="O53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P53" s="2">
+        <f>AVERAGE(H53,N53,O53)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>108842</v>
       </c>
@@ -4789,8 +5171,15 @@
       <c r="O54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54" s="2">
+        <f>AVERAGE(H54,N54,O54)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>103797</v>
       </c>
@@ -4836,8 +5225,15 @@
       <c r="O55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55">
+        <f>AVERAGE(H55,N55,O55)</f>
+        <v>8</v>
+      </c>
+      <c r="Q55" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>107777</v>
       </c>
@@ -4883,8 +5279,15 @@
       <c r="O56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56">
+        <f>AVERAGE(H56,N56,O56)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q56" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>107717</v>
       </c>
@@ -4930,8 +5333,15 @@
       <c r="O57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57">
+        <f>AVERAGE(H57,N57,O57)</f>
+        <v>9</v>
+      </c>
+      <c r="Q57" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>103443</v>
       </c>
@@ -4977,8 +5387,15 @@
       <c r="O58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58">
+        <f>AVERAGE(H58,N58,O58)</f>
+        <v>10</v>
+      </c>
+      <c r="Q58" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>108950</v>
       </c>
@@ -5024,8 +5441,15 @@
       <c r="O59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59">
+        <f>AVERAGE(H59,N59,O59)</f>
+        <v>12</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>108079</v>
       </c>
@@ -5071,8 +5495,15 @@
       <c r="O60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P60">
+        <f>AVERAGE(H60,N60,O60)</f>
+        <v>7</v>
+      </c>
+      <c r="Q60" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>109163</v>
       </c>
@@ -5118,8 +5549,15 @@
       <c r="O61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61" s="2">
+        <f>AVERAGE(H61,N61,O61)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q61" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>110347</v>
       </c>
@@ -5165,8 +5603,15 @@
       <c r="O62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62">
+        <f>AVERAGE(H62,N62,O62)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q62" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>109373</v>
       </c>
@@ -5212,8 +5657,15 @@
       <c r="O63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63">
+        <f>AVERAGE(H63,N63,O63)</f>
+        <v>10</v>
+      </c>
+      <c r="Q63" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>103203</v>
       </c>
@@ -5259,8 +5711,15 @@
       <c r="O64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64">
+        <f>AVERAGE(H64,N64,O64)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q64" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>107335</v>
       </c>
@@ -5306,8 +5765,15 @@
       <c r="O65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65">
+        <f>AVERAGE(H65,N65,O65)</f>
+        <v>11</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>93345</v>
       </c>
@@ -5353,8 +5819,15 @@
       <c r="O66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66">
+        <f>AVERAGE(H66,N66,O66)</f>
+        <v>12</v>
+      </c>
+      <c r="Q66" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>103409</v>
       </c>
@@ -5400,8 +5873,15 @@
       <c r="O67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P67">
+        <f>AVERAGE(H67,N67,O67)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q67" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>108105</v>
       </c>
@@ -5447,8 +5927,15 @@
       <c r="O68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" s="2">
+        <f>AVERAGE(H68,N68,O68)</f>
+        <v>10</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>107848</v>
       </c>
@@ -5494,8 +5981,15 @@
       <c r="O69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69">
+        <f>AVERAGE(H69,N69,O69)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q69" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>107318</v>
       </c>
@@ -5541,8 +6035,15 @@
       <c r="O70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70">
+        <f>AVERAGE(H70,N70,O70)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q70" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>107611</v>
       </c>
@@ -5588,8 +6089,15 @@
       <c r="O71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71">
+        <f>AVERAGE(H71,N71,O71)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q71" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>108845</v>
       </c>
@@ -5635,8 +6143,15 @@
       <c r="O72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P72">
+        <f>AVERAGE(H72,N72,O72)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q72" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>108098</v>
       </c>
@@ -5682,8 +6197,15 @@
       <c r="O73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P73">
+        <f>AVERAGE(H73,N73,O73)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q73" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>108723</v>
       </c>
@@ -5729,8 +6251,15 @@
       <c r="O74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P74">
+        <f>AVERAGE(H74,N74,O74)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q74" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>103757</v>
       </c>
@@ -5776,8 +6305,15 @@
       <c r="O75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P75">
+        <f>AVERAGE(H75,N75,O75)</f>
+        <v>8</v>
+      </c>
+      <c r="Q75" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>107396</v>
       </c>
@@ -5823,8 +6359,15 @@
       <c r="O76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P76">
+        <f>AVERAGE(H76,N76,O76)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>108675</v>
       </c>
@@ -5870,8 +6413,15 @@
       <c r="O77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P77">
+        <f>AVERAGE(H77,N77,O77)</f>
+        <v>8</v>
+      </c>
+      <c r="Q77" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>107584</v>
       </c>
@@ -5917,8 +6467,15 @@
       <c r="O78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P78">
+        <f>AVERAGE(H78,N78,O78)</f>
+        <v>9</v>
+      </c>
+      <c r="Q78" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>108329</v>
       </c>
@@ -5964,8 +6521,15 @@
       <c r="O79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P79">
+        <f>AVERAGE(H79,N79,O79)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q79" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>107874</v>
       </c>
@@ -6011,8 +6575,15 @@
       <c r="O80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80">
+        <f>AVERAGE(H80,N80,O80)</f>
+        <v>10</v>
+      </c>
+      <c r="Q80" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>107517</v>
       </c>
@@ -6058,8 +6629,15 @@
       <c r="O81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81">
+        <f>AVERAGE(H81,N81,O81)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q81" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>108513</v>
       </c>
@@ -6105,8 +6683,15 @@
       <c r="O82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82">
+        <f>AVERAGE(H82,N82,O82)</f>
+        <v>10</v>
+      </c>
+      <c r="Q82" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>104342</v>
       </c>
@@ -6152,8 +6737,15 @@
       <c r="O83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83">
+        <f>AVERAGE(H83,N83,O83)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q83" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>108752</v>
       </c>
@@ -6199,8 +6791,15 @@
       <c r="O84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84">
+        <f>AVERAGE(H84,N84,O84)</f>
+        <v>10</v>
+      </c>
+      <c r="Q84" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>103712</v>
       </c>
@@ -6246,8 +6845,15 @@
       <c r="O85">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85">
+        <f>AVERAGE(H85,N85,O85)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q85" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>108849</v>
       </c>
@@ -6293,8 +6899,15 @@
       <c r="O86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P86">
+        <f>AVERAGE(H86,N86,O86)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>108868</v>
       </c>
@@ -6340,8 +6953,15 @@
       <c r="O87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87" s="2">
+        <f>AVERAGE(H87,N87,O87)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q87" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>102380</v>
       </c>
@@ -6387,8 +7007,15 @@
       <c r="O88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88">
+        <f>AVERAGE(H88,N88,O88)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>107265</v>
       </c>
@@ -6434,8 +7061,15 @@
       <c r="O89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89">
+        <f>AVERAGE(H89,N89,O89)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>108280</v>
       </c>
@@ -6481,8 +7115,15 @@
       <c r="O90">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P90">
+        <f>AVERAGE(H90,N90,O90)</f>
+        <v>8</v>
+      </c>
+      <c r="Q90" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>97610</v>
       </c>
@@ -6528,8 +7169,15 @@
       <c r="O91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91" s="2">
+        <f>AVERAGE(H91,N91,O91)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q91" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>93316</v>
       </c>
@@ -6575,8 +7223,15 @@
       <c r="O92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92">
+        <f>AVERAGE(H92,N92,O92)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q92" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>110331</v>
       </c>
@@ -6622,8 +7277,15 @@
       <c r="O93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P93">
+        <f>AVERAGE(H93,N93,O93)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q93" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>104807</v>
       </c>
@@ -6669,8 +7331,15 @@
       <c r="O94">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94">
+        <f>AVERAGE(H94,N94,O94)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q94" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>108679</v>
       </c>
@@ -6716,8 +7385,15 @@
       <c r="O95">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P95">
+        <f>AVERAGE(H95,N95,O95)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q95" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>103028</v>
       </c>
@@ -6763,8 +7439,15 @@
       <c r="O96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96" s="2">
+        <f>AVERAGE(H96,N96,O96)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q96" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>105114</v>
       </c>
@@ -6810,8 +7493,15 @@
       <c r="O97">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P97">
+        <f>AVERAGE(H97,N97,O97)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q97" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>108800</v>
       </c>
@@ -6857,8 +7547,15 @@
       <c r="O98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P98" s="2">
+        <f>AVERAGE(H98,N98,O98)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q98" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>108050</v>
       </c>
@@ -6904,8 +7601,15 @@
       <c r="O99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P99">
+        <f>AVERAGE(H99,N99,O99)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q99" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>105491</v>
       </c>
@@ -6951,8 +7655,15 @@
       <c r="O100">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P100">
+        <f>AVERAGE(H100,N100,O100)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>102976</v>
       </c>
@@ -6998,8 +7709,15 @@
       <c r="O101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P101" s="2">
+        <f>AVERAGE(H101,N101,O101)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q101" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>108826</v>
       </c>
@@ -7045,8 +7763,15 @@
       <c r="O102">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P102">
+        <f>AVERAGE(H102,N102,O102)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>108436</v>
       </c>
@@ -7092,8 +7817,15 @@
       <c r="O103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P103" s="2">
+        <f>AVERAGE(H103,N103,O103)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q103" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>107233</v>
       </c>
@@ -7139,8 +7871,15 @@
       <c r="O104">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P104" s="2">
+        <f>AVERAGE(H104,N104,O104)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103167</v>
       </c>
@@ -7186,8 +7925,15 @@
       <c r="O105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P105">
+        <f>AVERAGE(H105,N105,O105)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q105" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>108760</v>
       </c>
@@ -7233,8 +7979,15 @@
       <c r="O106">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P106">
+        <f>AVERAGE(H106,N106,O106)</f>
+        <v>7</v>
+      </c>
+      <c r="Q106" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>103326</v>
       </c>
@@ -7280,8 +8033,15 @@
       <c r="O107">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P107" s="2">
+        <f>AVERAGE(H107,N107,O107)</f>
+        <v>10</v>
+      </c>
+      <c r="Q107" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>109152</v>
       </c>
@@ -7327,8 +8087,15 @@
       <c r="O108">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P108">
+        <f>AVERAGE(H108,N108,O108)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q108" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107895</v>
       </c>
@@ -7374,8 +8141,15 @@
       <c r="O109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P109">
+        <f>AVERAGE(H109,N109,O109)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q109" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>107267</v>
       </c>
@@ -7421,8 +8195,15 @@
       <c r="O110">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P110">
+        <f>AVERAGE(H110,N110,O110)</f>
+        <v>8</v>
+      </c>
+      <c r="Q110" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>103309</v>
       </c>
@@ -7468,8 +8249,15 @@
       <c r="O111">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P111">
+        <f>AVERAGE(H111,N111,O111)</f>
+        <v>9</v>
+      </c>
+      <c r="Q111" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>99440</v>
       </c>
@@ -7515,8 +8303,15 @@
       <c r="O112">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P112" s="2">
+        <f>AVERAGE(H112,N112,O112)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q112" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>93274</v>
       </c>
@@ -7562,8 +8357,15 @@
       <c r="O113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P113">
+        <f>AVERAGE(H113,N113,O113)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q113" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>102859</v>
       </c>
@@ -7609,8 +8411,15 @@
       <c r="O114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P114">
+        <f>AVERAGE(H114,N114,O114)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q114" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>104088</v>
       </c>
@@ -7656,8 +8465,15 @@
       <c r="O115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P115">
+        <f>AVERAGE(H115,N115,O115)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q115" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>102633</v>
       </c>
@@ -7703,8 +8519,15 @@
       <c r="O116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P116">
+        <f>AVERAGE(H116,N116,O116)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q116" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>108159</v>
       </c>
@@ -7750,8 +8573,15 @@
       <c r="O117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P117">
+        <f>AVERAGE(H117,N117,O117)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q117" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>108461</v>
       </c>
@@ -7797,8 +8627,15 @@
       <c r="O118">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P118" s="2">
+        <f>AVERAGE(H118,N118,O118)</f>
+        <v>10</v>
+      </c>
+      <c r="Q118" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>107635</v>
       </c>
@@ -7844,8 +8681,15 @@
       <c r="O119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P119">
+        <f>AVERAGE(H119,N119,O119)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="Q119" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>102716</v>
       </c>
@@ -7891,8 +8735,15 @@
       <c r="O120">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P120">
+        <f>AVERAGE(H120,N120,O120)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q120" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>107347</v>
       </c>
@@ -7938,8 +8789,15 @@
       <c r="O121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P121">
+        <f>AVERAGE(H121,N121,O121)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q121" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>110409</v>
       </c>
@@ -7985,8 +8843,15 @@
       <c r="O122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P122">
+        <f>AVERAGE(H122,N122,O122)</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="Q122" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>108540</v>
       </c>
@@ -8032,8 +8897,15 @@
       <c r="O123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P123" s="2">
+        <f>AVERAGE(H123,N123,O123)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q123" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>103112</v>
       </c>
@@ -8079,8 +8951,15 @@
       <c r="O124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P124">
+        <f>AVERAGE(H124,N124,O124)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q124" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>111224</v>
       </c>
@@ -8126,8 +9005,15 @@
       <c r="O125">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P125">
+        <f>AVERAGE(H125,N125,O125)</f>
+        <v>9</v>
+      </c>
+      <c r="Q125" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>102150</v>
       </c>
@@ -8173,8 +9059,15 @@
       <c r="O126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P126" s="2">
+        <f>AVERAGE(H126,N126,O126)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q126" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>107185</v>
       </c>
@@ -8220,8 +9113,15 @@
       <c r="O127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P127">
+        <f>AVERAGE(H127,N127,O127)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q127" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>104229</v>
       </c>
@@ -8267,8 +9167,15 @@
       <c r="O128">
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P128">
+        <f>AVERAGE(H128,N128,O128)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q128" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>103235</v>
       </c>
@@ -8314,8 +9221,15 @@
       <c r="O129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P129">
+        <f>AVERAGE(H129,N129,O129)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q129" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>110719</v>
       </c>
@@ -8361,8 +9275,15 @@
       <c r="O130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P130">
+        <f>AVERAGE(H130,N130,O130)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="Q130" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>102669</v>
       </c>
@@ -8408,8 +9329,15 @@
       <c r="O131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P131">
+        <f>AVERAGE(H131,N131,O131)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q131" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>108113</v>
       </c>
@@ -8455,8 +9383,15 @@
       <c r="O132">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P132">
+        <f>AVERAGE(H132,N132,O132)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q132" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>108204</v>
       </c>
@@ -8502,8 +9437,15 @@
       <c r="O133">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P133">
+        <f>AVERAGE(H133,N133,O133)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q133" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>107356</v>
       </c>
@@ -8549,8 +9491,15 @@
       <c r="O134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P134">
+        <f>AVERAGE(H134,N134,O134)</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Q134" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>102011</v>
       </c>
@@ -8596,8 +9545,15 @@
       <c r="O135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P135">
+        <f>AVERAGE(H135,N135,O135)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q135" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>104183</v>
       </c>
@@ -8643,8 +9599,15 @@
       <c r="O136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P136">
+        <f>AVERAGE(H136,N136,O136)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q136" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>108629</v>
       </c>
@@ -8690,8 +9653,15 @@
       <c r="O137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P137">
+        <f>AVERAGE(H137,N137,O137)</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Q137" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>102743</v>
       </c>
@@ -8737,8 +9707,15 @@
       <c r="O138">
         <v>2</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P138" s="2">
+        <f>AVERAGE(H138,N138,O138)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q138" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>108654</v>
       </c>
@@ -8784,8 +9761,15 @@
       <c r="O139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P139">
+        <f>AVERAGE(H139,N139,O139)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q139" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>108869</v>
       </c>
@@ -8831,8 +9815,15 @@
       <c r="O140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P140">
+        <f>AVERAGE(H140,N140,O140)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q140" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>103761</v>
       </c>
@@ -8878,8 +9869,15 @@
       <c r="O141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P141" s="2">
+        <f>AVERAGE(H141,N141,O141)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q141" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>107208</v>
       </c>
@@ -8925,8 +9923,15 @@
       <c r="O142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P142">
+        <f>AVERAGE(H142,N142,O142)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="Q142" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>103314</v>
       </c>
@@ -8972,8 +9977,15 @@
       <c r="O143">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P143" s="2">
+        <f>AVERAGE(H143,N143,O143)</f>
+        <v>8</v>
+      </c>
+      <c r="Q143" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>109150</v>
       </c>
@@ -9019,8 +10031,15 @@
       <c r="O144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P144">
+        <f>AVERAGE(H144,N144,O144)</f>
+        <v>10</v>
+      </c>
+      <c r="Q144" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>105431</v>
       </c>
@@ -9066,8 +10085,15 @@
       <c r="O145">
         <v>2</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P145" s="2">
+        <f>AVERAGE(H145,N145,O145)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q145" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>103768</v>
       </c>
@@ -9113,8 +10139,15 @@
       <c r="O146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P146">
+        <f>AVERAGE(H146,N146,O146)</f>
+        <v>11</v>
+      </c>
+      <c r="Q146" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>98007</v>
       </c>
@@ -9160,8 +10193,15 @@
       <c r="O147">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P147">
+        <f>AVERAGE(H147,N147,O147)</f>
+        <v>7</v>
+      </c>
+      <c r="Q147" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>107594</v>
       </c>
@@ -9207,8 +10247,15 @@
       <c r="O148">
         <v>2</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P148">
+        <f>AVERAGE(H148,N148,O148)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q148" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>107319</v>
       </c>
@@ -9254,8 +10301,15 @@
       <c r="O149">
         <v>2</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P149">
+        <f>AVERAGE(H149,N149,O149)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="Q149" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>99397</v>
       </c>
@@ -9301,8 +10355,15 @@
       <c r="O150">
         <v>2</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P150">
+        <f>AVERAGE(H150,N150,O150)</f>
+        <v>9</v>
+      </c>
+      <c r="Q150" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>105127</v>
       </c>
@@ -9348,8 +10409,15 @@
       <c r="O151">
         <v>2</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P151" s="2">
+        <f>AVERAGE(H151,N151,O151)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q151" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>105083</v>
       </c>
@@ -9395,8 +10463,15 @@
       <c r="O152">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P152" s="2">
+        <f>AVERAGE(H152,N152,O152)</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q152" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>109162</v>
       </c>
@@ -9442,8 +10517,15 @@
       <c r="O153">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P153">
+        <f>AVERAGE(H153,N153,O153)</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="Q153" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>108225</v>
       </c>
@@ -9489,8 +10571,15 @@
       <c r="O154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P154">
+        <f>AVERAGE(H154,N154,O154)</f>
+        <v>6</v>
+      </c>
+      <c r="Q154" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105880</v>
       </c>
@@ -9536,8 +10625,15 @@
       <c r="O155">
         <v>2</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P155">
+        <f>AVERAGE(H155,N155,O155)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q155" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>108078</v>
       </c>
@@ -9583,8 +10679,15 @@
       <c r="O156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P156">
+        <f>AVERAGE(H156,N156,O156)</f>
+        <v>10</v>
+      </c>
+      <c r="Q156" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>108146</v>
       </c>
@@ -9630,8 +10733,15 @@
       <c r="O157">
         <v>2</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P157" s="2">
+        <f>AVERAGE(H157,N157,O157)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q157" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>102437</v>
       </c>
@@ -9677,8 +10787,15 @@
       <c r="O158">
         <v>2</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P158">
+        <f>AVERAGE(H158,N158,O158)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="Q158" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>97876</v>
       </c>
@@ -9724,8 +10841,15 @@
       <c r="O159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P159">
+        <f>AVERAGE(H159,N159,O159)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="Q159" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>103910</v>
       </c>
@@ -9770,6 +10894,13 @@
       </c>
       <c r="O160">
         <v>2</v>
+      </c>
+      <c r="P160">
+        <f>AVERAGE(H160,N160,O160)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="Q160" s="5" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>